<commit_message>
updataed graphs for random player playing against learned weight, learned weights has a high percentage of wins when it's white
</commit_message>
<xml_diff>
--- a/reversi_othello/game_analysis.xlsx
+++ b/reversi_othello/game_analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="0" windowWidth="17256" windowHeight="7008"/>
+    <workbookView xWindow="3744" yWindow="0" windowWidth="17256" windowHeight="7008"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,13 +77,13 @@
     <t>increase the weight by 1 and at the other positions, decrease it by 1. Nothing to be done at tie positions</t>
   </si>
   <si>
-    <t>When one of the weights is played against a random player, the results are still equal, ie, the machine player using</t>
+    <t>More tweaking is required to incorporate the state of the game into updating the decisions.</t>
   </si>
   <si>
-    <t>learned wights shows no superiority over a random player.</t>
+    <t>When one of the weights is played against a random player, the results are quite suprising as whoever's white seems to</t>
   </si>
   <si>
-    <t>More tweaking is required to incorporate the state of the game into updating the decisions.</t>
+    <t>winning a lot of games, need to check what happens if the comp player is always white</t>
   </si>
 </sst>
 </file>
@@ -649,22 +649,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>567267</xdr:colOff>
+      <xdr:colOff>211666</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>62088</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
-      <xdr:colOff>313267</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>84668</xdr:rowOff>
+      <xdr:colOff>474133</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B3877C9-1616-4E33-B80D-500418E72D90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40ADF6B5-A5A4-4AE8-8355-DCEF812969DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -686,8 +686,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20074467" y="0"/>
-          <a:ext cx="7670800" cy="5113868"/>
+          <a:off x="19718866" y="62088"/>
+          <a:ext cx="8187267" cy="5458178"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -998,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI609"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AX39" sqref="AX39"/>
+    <sheetView tabSelected="1" topLeftCell="AB17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AH38" sqref="AH38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3242,7 +3242,7 @@
         <v>-52</v>
       </c>
       <c r="AH36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.3">
@@ -3319,7 +3319,7 @@
         <v>74</v>
       </c>
       <c r="AH37" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.3">
@@ -3396,7 +3396,7 @@
         <v>-34</v>
       </c>
       <c r="AH38" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.3">
@@ -27499,18 +27499,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="S21:Z21"/>
+    <mergeCell ref="S31:Z31"/>
+    <mergeCell ref="S41:Z41"/>
+    <mergeCell ref="S51:Z51"/>
+    <mergeCell ref="J1:Q1"/>
     <mergeCell ref="S61:Z61"/>
     <mergeCell ref="S71:Z71"/>
     <mergeCell ref="S81:Z81"/>
     <mergeCell ref="S91:Z91"/>
     <mergeCell ref="S1:Z1"/>
     <mergeCell ref="S11:Z11"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="S21:Z21"/>
-    <mergeCell ref="S31:Z31"/>
-    <mergeCell ref="S41:Z41"/>
-    <mergeCell ref="S51:Z51"/>
-    <mergeCell ref="J1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="S32:Z39">
     <cfRule type="colorScale" priority="11">

</xml_diff>

<commit_message>
updated graphs for matches between random player and the computer player, made the corresponding corrections in the code to prepare the correct graphs
</commit_message>
<xml_diff>
--- a/reversi_othello/game_analysis.xlsx
+++ b/reversi_othello/game_analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3744" yWindow="0" windowWidth="17256" windowHeight="7008"/>
+    <workbookView xWindow="4680" yWindow="0" windowWidth="17256" windowHeight="7008"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Weights Sim 2</t>
   </si>
@@ -80,10 +80,13 @@
     <t>More tweaking is required to incorporate the state of the game into updating the decisions.</t>
   </si>
   <si>
-    <t>When one of the weights is played against a random player, the results are quite suprising as whoever's white seems to</t>
+    <t>When one of the weights is played against a random player, the results are quite good as majority of the time</t>
   </si>
   <si>
-    <t>winning a lot of games, need to check what happens if the comp player is always white</t>
+    <t>the machine player with the learned weights is winning, so, in effect something has been learned, although not quite good enough</t>
+  </si>
+  <si>
+    <t>A decision tree of future game states might perform better, this learned weights player could be useful for teaching a neural network</t>
   </si>
 </sst>
 </file>
@@ -649,22 +652,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>211666</xdr:colOff>
+      <xdr:colOff>541867</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>62088</xdr:rowOff>
+      <xdr:rowOff>172154</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
-      <xdr:colOff>474133</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>118533</xdr:rowOff>
+      <xdr:colOff>436035</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>169332</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40ADF6B5-A5A4-4AE8-8355-DCEF812969DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB0E1C61-5A7E-44BF-8880-C09F2CD69587}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -686,8 +689,58 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19718866" y="62088"/>
-          <a:ext cx="8187267" cy="5458178"/>
+          <a:off x="20049067" y="172154"/>
+          <a:ext cx="7818968" cy="5212645"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>135465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>118532</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{694BC637-BEB2-4D0D-9ECC-6F1741B63ED8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20066000" y="5164665"/>
+          <a:ext cx="7797800" cy="5198534"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -998,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI609"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AH38" sqref="AH38"/>
+    <sheetView tabSelected="1" topLeftCell="AB37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AH67" sqref="AH67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2856,9 +2909,6 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
-      <c r="AH31" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -2933,11 +2983,8 @@
       <c r="Z32">
         <v>183</v>
       </c>
-      <c r="AH32" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
@@ -3010,11 +3057,8 @@
       <c r="Z33">
         <v>13</v>
       </c>
-      <c r="AH33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>0</v>
       </c>
@@ -3087,11 +3131,8 @@
       <c r="Z34">
         <v>-70</v>
       </c>
-      <c r="AH34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>0</v>
       </c>
@@ -3164,11 +3205,8 @@
       <c r="Z35">
         <v>66</v>
       </c>
-      <c r="AH35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0</v>
       </c>
@@ -3241,11 +3279,8 @@
       <c r="Z36">
         <v>-52</v>
       </c>
-      <c r="AH36" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0</v>
       </c>
@@ -3318,11 +3353,8 @@
       <c r="Z37">
         <v>74</v>
       </c>
-      <c r="AH37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0</v>
       </c>
@@ -3395,11 +3427,8 @@
       <c r="Z38">
         <v>-34</v>
       </c>
-      <c r="AH38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0</v>
       </c>
@@ -3473,7 +3502,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="S41" s="2" t="s">
         <v>3</v>
       </c>
@@ -3485,7 +3514,7 @@
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>0</v>
       </c>
@@ -3559,7 +3588,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0</v>
       </c>
@@ -3633,7 +3662,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>0</v>
       </c>
@@ -3707,7 +3736,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>0</v>
       </c>
@@ -3781,7 +3810,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>0</v>
       </c>
@@ -3855,7 +3884,7 @@
         <v>-175</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>0</v>
       </c>
@@ -3929,7 +3958,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>0</v>
       </c>
@@ -4003,7 +4032,7 @@
         <v>-191</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0</v>
       </c>
@@ -4077,7 +4106,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="S51" s="2" t="s">
         <v>4</v>
       </c>
@@ -4089,7 +4118,7 @@
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0</v>
       </c>
@@ -4163,7 +4192,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>0</v>
       </c>
@@ -4237,7 +4266,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>0</v>
       </c>
@@ -4311,7 +4340,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>0</v>
       </c>
@@ -4385,7 +4414,7 @@
         <v>-37</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>0</v>
       </c>
@@ -4459,7 +4488,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>0</v>
       </c>
@@ -4533,7 +4562,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>0</v>
       </c>
@@ -4606,8 +4635,11 @@
       <c r="Z58">
         <v>-32</v>
       </c>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AH58" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>0</v>
       </c>
@@ -4680,8 +4712,16 @@
       <c r="Z59">
         <v>184</v>
       </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AH59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="AH60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
       <c r="S61" s="2" t="s">
         <v>5</v>
       </c>
@@ -4692,8 +4732,11 @@
       <c r="X61" s="2"/>
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AH61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>0</v>
       </c>
@@ -4766,8 +4809,11 @@
       <c r="Z62">
         <v>272</v>
       </c>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AH62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>0</v>
       </c>
@@ -4840,8 +4886,11 @@
       <c r="Z63">
         <v>42</v>
       </c>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AH63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>0</v>
       </c>
@@ -4914,8 +4963,11 @@
       <c r="Z64">
         <v>-69</v>
       </c>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AH64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>0</v>
       </c>
@@ -4988,8 +5040,11 @@
       <c r="Z65">
         <v>87</v>
       </c>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AH65" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>0</v>
       </c>
@@ -5062,8 +5117,11 @@
       <c r="Z66">
         <v>23</v>
       </c>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AH66" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>0</v>
       </c>
@@ -5137,7 +5195,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>0</v>
       </c>
@@ -5211,7 +5269,7 @@
         <v>-85</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>0</v>
       </c>
@@ -5285,7 +5343,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.3">
       <c r="S71" s="2" t="s">
         <v>6</v>
       </c>
@@ -5297,7 +5355,7 @@
       <c r="Y71" s="2"/>
       <c r="Z71" s="2"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>0</v>
       </c>
@@ -5371,7 +5429,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>0</v>
       </c>
@@ -5445,7 +5503,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>0</v>
       </c>
@@ -5519,7 +5577,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>0</v>
       </c>
@@ -5593,7 +5651,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>-1</v>
       </c>
@@ -5667,7 +5725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>0</v>
       </c>
@@ -5741,7 +5799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>0</v>
       </c>
@@ -5815,7 +5873,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>0</v>
       </c>
@@ -27499,18 +27557,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="S61:Z61"/>
+    <mergeCell ref="S71:Z71"/>
+    <mergeCell ref="S81:Z81"/>
+    <mergeCell ref="S91:Z91"/>
+    <mergeCell ref="S1:Z1"/>
+    <mergeCell ref="S11:Z11"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="S21:Z21"/>
     <mergeCell ref="S31:Z31"/>
     <mergeCell ref="S41:Z41"/>
     <mergeCell ref="S51:Z51"/>
     <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="S61:Z61"/>
-    <mergeCell ref="S71:Z71"/>
-    <mergeCell ref="S81:Z81"/>
-    <mergeCell ref="S91:Z91"/>
-    <mergeCell ref="S1:Z1"/>
-    <mergeCell ref="S11:Z11"/>
   </mergeCells>
   <conditionalFormatting sqref="S32:Z39">
     <cfRule type="colorScale" priority="11">

</xml_diff>